<commit_message>
campos de compra automatizados
</commit_message>
<xml_diff>
--- a/data/inventario_minsalBaseOriginal.xlsx
+++ b/data/inventario_minsalBaseOriginal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sistema_inventariosMinsal\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6381E6C2-164D-4F0A-9A96-8C9E6459B386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E9AFF5-A635-4367-AE90-5B72D5A9BC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{33EF6376-3F5A-46D1-9B87-DA96CC38AB62}"/>
+    <workbookView xWindow="36" yWindow="1884" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{33EF6376-3F5A-46D1-9B87-DA96CC38AB62}"/>
   </bookViews>
   <sheets>
     <sheet name="Catálogo" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="231">
   <si>
     <t>Código</t>
   </si>
@@ -602,12 +602,6 @@
     <t>01/07/2027</t>
   </si>
   <si>
-    <t>20/07/2025</t>
-  </si>
-  <si>
-    <t>20/07/2027</t>
-  </si>
-  <si>
     <t>10/08/2025</t>
   </si>
   <si>
@@ -752,9 +746,6 @@
     <t>Donación</t>
   </si>
   <si>
-    <t>Cantidad Despachada</t>
-  </si>
-  <si>
     <t>Cant_Actual</t>
   </si>
   <si>
@@ -762,6 +753,9 @@
   </si>
   <si>
     <t>Presentacion</t>
+  </si>
+  <si>
+    <t>Cantidad_Despachada</t>
   </si>
 </sst>
 </file>
@@ -771,7 +765,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -925,13 +919,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1257,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FD917-88A1-4BCB-B444-9B25C23BB9C3}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1277,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1948,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCC6A64-6EEC-4F9D-92CD-772FEB3A9BD0}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1985,7 +1979,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G1" s="26" t="s">
         <v>13</v>
@@ -1997,7 +1991,7 @@
         <v>15</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2047,7 +2041,7 @@
         <v>Paracetamol</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E3" s="10">
         <v>500</v>
@@ -2117,7 +2111,7 @@
         <v>Omeprazol</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E5" s="10">
         <v>10000</v>
@@ -2580,11 +2574,11 @@
       <c r="F18">
         <v>7900</v>
       </c>
-      <c r="G18" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>180</v>
+      <c r="G18" s="26">
+        <v>45950</v>
+      </c>
+      <c r="H18" s="26">
+        <v>45981</v>
       </c>
       <c r="I18" s="11">
         <f>VLOOKUP(B18,Catálogo!A:F,5,FALSE)</f>
@@ -2592,7 +2586,7 @@
       </c>
       <c r="J18" s="10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>✅ Activo</v>
+        <v>⚠️ Por Vencer</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2616,10 +2610,10 @@
         <v>5900</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I19" s="11">
         <f>VLOOKUP(B19,Catálogo!A:F,5,FALSE)</f>
@@ -2651,7 +2645,7 @@
         <v>6700</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H20" s="26">
         <v>45915</v>
@@ -2686,10 +2680,10 @@
         <v>3900</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I21" s="11">
         <f>VLOOKUP(B21,Catálogo!A:F,5,FALSE)</f>
@@ -2771,10 +2765,10 @@
         <v>96</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>11</v>
@@ -2878,7 +2872,7 @@
         <v xml:space="preserve">Compra Nacional </v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J3" s="6">
         <f>VLOOKUP(I3,Inventario_Lotes!$D:$J,2,FALSE)</f>
@@ -2959,10 +2953,10 @@
         <v>45809</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>51</v>
@@ -2984,7 +2978,7 @@
         <v xml:space="preserve">Compra Nacional </v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J5" s="6">
         <f>VLOOKUP(I5,Inventario_Lotes!$D:$J,2,FALSE)</f>
@@ -3012,10 +3006,10 @@
         <v>45723</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>54</v>
@@ -3065,10 +3059,10 @@
         <v>45787</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>57</v>
@@ -3118,10 +3112,10 @@
         <v>45666</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>60</v>
@@ -3171,10 +3165,10 @@
         <v>45856</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>63</v>
@@ -3224,10 +3218,10 @@
         <v>45891</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>106</v>
@@ -3277,10 +3271,10 @@
         <v>45895</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>111</v>
@@ -3330,10 +3324,10 @@
         <v>45898</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>112</v>
@@ -3383,10 +3377,10 @@
         <v>45900</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>113</v>
@@ -3436,10 +3430,10 @@
         <v>45901</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>114</v>
@@ -3489,10 +3483,10 @@
         <v>45904</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>115</v>
@@ -3542,10 +3536,10 @@
         <v>45690</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>116</v>
@@ -3595,10 +3589,10 @@
         <v>45908</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>117</v>
@@ -3648,10 +3642,10 @@
         <v>45925</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>118</v>
@@ -3666,7 +3660,7 @@
       </c>
       <c r="G18" t="str">
         <f ca="1">IFERROR(VLOOKUP(I18,Inventario_Lotes!$D:$J,7,FALSE),"No encontrado")</f>
-        <v>✅ Activo</v>
+        <v>⚠️ Por Vencer</v>
       </c>
       <c r="H18" t="str">
         <f>IFERROR(VLOOKUP(C18,Proveedores!$A$2:$B$50,2,FALSE),"Definir")</f>
@@ -3701,10 +3695,10 @@
         <v>45931</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>119</v>
@@ -3754,10 +3748,10 @@
         <v>45934</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>120</v>
@@ -3807,10 +3801,10 @@
         <v>45956</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>121</v>
@@ -4010,8 +4004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953FA125-C20F-4A67-8AC4-5554B9900DC5}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4048,7 +4042,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>15</v>
@@ -4081,7 +4075,7 @@
         <v>67</v>
       </c>
       <c r="G2" s="6">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H2" s="21">
         <f>IFERROR(VLOOKUP(TRIM(F2),Inventario_Lotes!D:I,6,FALSE),"❌ No encontrado")</f>
@@ -4089,7 +4083,7 @@
       </c>
       <c r="I2" s="13">
         <f>IFERROR(G2*H2,"")</f>
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>84</v>
@@ -4102,18 +4096,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="466" yWindow="398" count="1">
-        <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD587928-2E3C-40ED-A578-3472C073F8DF}">
-          <x14:formula1>
-            <xm:f>IFERROR(G2&lt;=VLOOKUP(D2,Catálogo!$A:$I,9,FALSE),TRUE)</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4248,7 +4230,7 @@
       </c>
       <c r="F10" s="2">
         <f>IFERROR(VLOOKUP(E10,Libro_Salidas!D:I,6,FALSE),0)</f>
-        <v>6000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -4269,7 +4251,7 @@
       </c>
       <c r="G11" s="14">
         <f>IFERROR(VLOOKUP(E11,Libro_Salidas!D:I,6,FALSE),0)</f>
-        <v>6000</v>
+        <v>12000</v>
       </c>
     </row>
   </sheetData>
@@ -4371,11 +4353,11 @@
       </c>
       <c r="E5" s="2">
         <f>IFERROR(VLOOKUP(B5,Libro_Salidas!A:J,9,FALSE),0)</f>
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="F5" s="22">
         <f xml:space="preserve"> F4 + D5 - E5</f>
-        <v>34000</v>
+        <v>28000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -4387,7 +4369,7 @@
       </c>
       <c r="F7" s="23" cm="1">
         <f t="array" ref="F7">LOOKUP(2,1/(VALUE(F3:F6)&lt;&gt;0),VALUE(F3:F6))</f>
-        <v>34000</v>
+        <v>28000</v>
       </c>
     </row>
   </sheetData>
@@ -5075,7 +5057,7 @@
       </c>
       <c r="D36" t="str">
         <f ca="1">IF(B36&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B36,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B36,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>Lote vence el 01/08/jueves (-452 días)</v>
+        <v>Lote vence el 01/08/jueves (-453 días)</v>
       </c>
       <c r="E36" t="str">
         <f ca="1">IF(B36&lt;&gt;"","⚠️ USAR PRIORITARIAMENTE","")</f>
@@ -5159,7 +5141,7 @@
       </c>
       <c r="D40" t="str">
         <f ca="1">IF(B40&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B40,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B40,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>Lote vence el 10/11/lunes (14 días)</v>
+        <v>Lote vence el 10/11/lunes (13 días)</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -5397,10 +5379,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5408,7 +5390,7 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5416,7 +5398,7 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5424,143 +5406,143 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>